<commit_message>
modified processChapters & added tests
</commit_message>
<xml_diff>
--- a/files/output/Comparison_FPROG.xlsx
+++ b/files/output/Comparison_FPROG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fhtw-my.sharepoint.com/personal/if21b028_technikum-wien_at/Documents/INFORMATIK/Semester 5/FPROG/project/FPROG/files/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="104" documentId="8_{BBED4159-DCCB-4A4C-8A89-83957CA5B522}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E55AEBC6-8D6C-428F-AC2D-6761E38BA0E1}"/>
+  <xr:revisionPtr revIDLastSave="118" documentId="8_{BBED4159-DCCB-4A4C-8A89-83957CA5B522}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{804DBE43-B364-41CE-AD53-A7886D5EF1CD}"/>
   <bookViews>
     <workbookView xWindow="3495" yWindow="960" windowWidth="21600" windowHeight="11385" xr2:uid="{CD60B827-A9D0-4185-BC28-64C39489518C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="497">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="455">
   <si>
     <t>Chapter 1: peace-related</t>
   </si>
@@ -1136,21 +1136,9 @@
     <t>Chapter 9: peace-related</t>
   </si>
   <si>
-    <t>Chapter 32: peace-related</t>
-  </si>
-  <si>
-    <t>Chapter 50: peace-related</t>
-  </si>
-  <si>
-    <t>Chapter 69: peace-related</t>
-  </si>
-  <si>
     <t>Chapter 82: peace-related</t>
   </si>
   <si>
-    <t>Chapter 94: peace-related</t>
-  </si>
-  <si>
     <t>Chapter 108: peace-related</t>
   </si>
   <si>
@@ -1163,21 +1151,9 @@
     <t>Chapter 139: peace-related</t>
   </si>
   <si>
-    <t>Chapter 169: peace-related</t>
-  </si>
-  <si>
-    <t>Chapter 193: peace-related</t>
-  </si>
-  <si>
     <t>Chapter 203: peace-related</t>
   </si>
   <si>
-    <t>Chapter 235: peace-related</t>
-  </si>
-  <si>
-    <t>Chapter 308: peace-related</t>
-  </si>
-  <si>
     <t>Moodle Lösung</t>
   </si>
   <si>
@@ -1187,51 +1163,24 @@
     <t>Match</t>
   </si>
   <si>
-    <t>Chapter 29: war-related</t>
-  </si>
-  <si>
-    <t>Chapter 100: war-related</t>
-  </si>
-  <si>
     <t>Chapter 238: war-related</t>
   </si>
   <si>
     <t>Chapter 284: war-related</t>
   </si>
   <si>
-    <t>Chapter 354: war-related</t>
-  </si>
-  <si>
-    <t>Chapter 20: peace-related</t>
-  </si>
-  <si>
     <t>Chapter 26: peace-related</t>
   </si>
   <si>
-    <t>Chapter 76: peace-related</t>
-  </si>
-  <si>
     <t>Chapter 143: peace-related</t>
   </si>
   <si>
     <t>Chapter 144: peace-related</t>
   </si>
   <si>
-    <t>Chapter 153: peace-related</t>
-  </si>
-  <si>
-    <t>Chapter 184: peace-related</t>
-  </si>
-  <si>
     <t>Chapter 187: peace-related</t>
   </si>
   <si>
-    <t>Chapter 277: peace-related</t>
-  </si>
-  <si>
-    <t>Chapter 334: peace-related</t>
-  </si>
-  <si>
     <t>Chapter 352: peace-related</t>
   </si>
   <si>
@@ -1262,24 +1211,12 @@
     <t>Moodle</t>
   </si>
   <si>
-    <t>Chapter 27: war-related</t>
-  </si>
-  <si>
     <t>Chapter 43: war-related</t>
   </si>
   <si>
-    <t>Chapter 52: war-related</t>
-  </si>
-  <si>
-    <t>Chapter 57: war-related</t>
-  </si>
-  <si>
     <t>Chapter 58: war-related</t>
   </si>
   <si>
-    <t>Chapter 75: war-related</t>
-  </si>
-  <si>
     <t>Chapter 83: peace-related</t>
   </si>
   <si>
@@ -1292,63 +1229,33 @@
     <t>Chapter 103: war-related</t>
   </si>
   <si>
-    <t>Chapter 117: war-related</t>
-  </si>
-  <si>
-    <t>Chapter 118: peace-related</t>
-  </si>
-  <si>
     <t>Chapter 122: peace-related</t>
   </si>
   <si>
     <t>Chapter 133: peace-related</t>
   </si>
   <si>
-    <t>Chapter 137: war-related</t>
-  </si>
-  <si>
-    <t>Chapter 152: war-related</t>
-  </si>
-  <si>
     <t>Chapter 175: war-related</t>
   </si>
   <si>
-    <t>Chapter 181: war-related</t>
-  </si>
-  <si>
-    <t>Chapter 185: war-related</t>
-  </si>
-  <si>
-    <t>Chapter 189: war-related</t>
-  </si>
-  <si>
     <t>Chapter 195: war-related</t>
   </si>
   <si>
     <t>Chapter 207: war-related</t>
   </si>
   <si>
-    <t>Chapter 209: war-related</t>
-  </si>
-  <si>
     <t>Chapter 215: war-related</t>
   </si>
   <si>
     <t>Chapter 231: war-related</t>
   </si>
   <si>
-    <t>Chapter 236: war-related</t>
-  </si>
-  <si>
     <t>Chapter 241: war-related</t>
   </si>
   <si>
     <t>Chapter 255: war-related</t>
   </si>
   <si>
-    <t>Chapter 262: war-related</t>
-  </si>
-  <si>
     <t>Chapter 263: war-related</t>
   </si>
   <si>
@@ -1358,141 +1265,36 @@
     <t>Chapter 305: war-related</t>
   </si>
   <si>
-    <t>Chapter 312: war-related</t>
-  </si>
-  <si>
     <t>Chapter 321: war-related</t>
   </si>
   <si>
-    <t>Chapter 333: war-related</t>
-  </si>
-  <si>
-    <t>Chapter 339: war-related</t>
-  </si>
-  <si>
-    <t>Chapter 365: war-related</t>
-  </si>
-  <si>
-    <t>Chapter 8: peace-related</t>
-  </si>
-  <si>
     <t>Chapter 24: peace-related</t>
   </si>
   <si>
     <t>Chapter 345: peace-related</t>
   </si>
   <si>
-    <t>Chapter 361: peace-related</t>
-  </si>
-  <si>
-    <t>Chapter 89: war-related</t>
-  </si>
-  <si>
-    <t>Chapter 168: war-related</t>
-  </si>
-  <si>
-    <t>Chapter 170: war-related</t>
-  </si>
-  <si>
-    <t>Chapter 205: war-related</t>
-  </si>
-  <si>
-    <t>Chapter 227: peace-related</t>
-  </si>
-  <si>
-    <t>Chapter 228: war-related</t>
-  </si>
-  <si>
-    <t>Chapter 240: war-related</t>
-  </si>
-  <si>
-    <t>Chapter 248: war-related</t>
-  </si>
-  <si>
-    <t>Chapter 274: war-related</t>
-  </si>
-  <si>
-    <t>Chapter 10: war-related</t>
-  </si>
-  <si>
-    <t>Chapter 162: war-related</t>
-  </si>
-  <si>
     <t>Chapter 174: war-related</t>
   </si>
   <si>
-    <t>Chapter 320: war-related</t>
-  </si>
-  <si>
-    <t>Chapter 111: peace-related</t>
-  </si>
-  <si>
     <t>Chapter 115: peace-related</t>
   </si>
   <si>
-    <t>Chapter 180: peace-related</t>
-  </si>
-  <si>
-    <t>Chapter 319: peace-related</t>
-  </si>
-  <si>
-    <t>Chapter 342: peace-related</t>
-  </si>
-  <si>
-    <t>Chapter 33: war-related</t>
-  </si>
-  <si>
-    <t>Chapter 110: war-related</t>
-  </si>
-  <si>
     <t>Chapter 222: war-related</t>
   </si>
   <si>
-    <t>Chapter 292: war-related</t>
-  </si>
-  <si>
     <t>Chapter 315: war-related</t>
   </si>
   <si>
-    <t>Chapter 358: war-related</t>
-  </si>
-  <si>
-    <t>Chapter 28: peace-related</t>
-  </si>
-  <si>
-    <t>Chapter 86: peace-related</t>
-  </si>
-  <si>
-    <t>Chapter 106: peace-related</t>
-  </si>
-  <si>
-    <t>Chapter 245: war-related</t>
-  </si>
-  <si>
-    <t>Chapter 270: war-related</t>
-  </si>
-  <si>
-    <t>Chapter 272: war-related</t>
-  </si>
-  <si>
     <t>Chapter 343: peace-related</t>
   </si>
   <si>
-    <t>Chapter 77: war-related</t>
-  </si>
-  <si>
     <t>Chapter 302: war-related</t>
   </si>
   <si>
-    <t>Chapter 309: war-related</t>
-  </si>
-  <si>
     <t>Chapter 126: peace-related</t>
   </si>
   <si>
-    <t>Chapter 138: peace-related</t>
-  </si>
-  <si>
     <t>Chapter 177: war-related</t>
   </si>
   <si>
@@ -1502,31 +1304,103 @@
     <t>Chapter 201: peace-related</t>
   </si>
   <si>
-    <t>Chapter 239: peace-related</t>
-  </si>
-  <si>
     <t>Chapter 288: war-related</t>
   </si>
   <si>
-    <t>Chapter 357: peace-related</t>
-  </si>
-  <si>
-    <t>Chapter 13: war-related</t>
-  </si>
-  <si>
-    <t>Chapter 85: war-related</t>
-  </si>
-  <si>
-    <t>Chapter 194: war-related</t>
-  </si>
-  <si>
-    <t>Chapter 294: peace-related</t>
-  </si>
-  <si>
     <t>Chapter 304: war-related</t>
   </si>
   <si>
-    <t>Chapter 348: war-related</t>
+    <t>Chapter 7: peace-related</t>
+  </si>
+  <si>
+    <t>Chapter 11: war-related</t>
+  </si>
+  <si>
+    <t>Chapter 14: war-related</t>
+  </si>
+  <si>
+    <t>Chapter 19: peace-related</t>
+  </si>
+  <si>
+    <t>Chapter 54: war-related</t>
+  </si>
+  <si>
+    <t>Chapter 71: peace-related</t>
+  </si>
+  <si>
+    <t>Chapter 72: war-related</t>
+  </si>
+  <si>
+    <t>Chapter 78: war-related</t>
+  </si>
+  <si>
+    <t>Chapter 128: peace-related</t>
+  </si>
+  <si>
+    <t>Chapter 129: war-related</t>
+  </si>
+  <si>
+    <t>Chapter 131: peace-related</t>
+  </si>
+  <si>
+    <t>Chapter 132: war-related</t>
+  </si>
+  <si>
+    <t>Chapter 163: war-related</t>
+  </si>
+  <si>
+    <t>Chapter 186: war-related</t>
+  </si>
+  <si>
+    <t>Chapter 200: war-related</t>
+  </si>
+  <si>
+    <t>Chapter 208: war-related</t>
+  </si>
+  <si>
+    <t>Chapter 242: war-related</t>
+  </si>
+  <si>
+    <t>Chapter 246: war-related</t>
+  </si>
+  <si>
+    <t>Chapter 251: war-related</t>
+  </si>
+  <si>
+    <t>Chapter 253: peace-related</t>
+  </si>
+  <si>
+    <t>Chapter 256: war-related</t>
+  </si>
+  <si>
+    <t>Chapter 269: war-related</t>
+  </si>
+  <si>
+    <t>Chapter 271: war-related</t>
+  </si>
+  <si>
+    <t>Chapter 273: war-related</t>
+  </si>
+  <si>
+    <t>Chapter 279: peace-related</t>
+  </si>
+  <si>
+    <t>Chapter 291: war-related</t>
+  </si>
+  <si>
+    <t>Chapter 295: peace-related</t>
+  </si>
+  <si>
+    <t>Chapter 311: war-related</t>
+  </si>
+  <si>
+    <t>Chapter 330: war-related</t>
+  </si>
+  <si>
+    <t>Chapter 349: war-related</t>
+  </si>
+  <si>
+    <t>Chapter 366: war-related</t>
   </si>
 </sst>
 </file>
@@ -1895,6 +1769,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
@@ -2196,7 +2074,7 @@
   <dimension ref="A1:G369"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2209,13 +2087,13 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1">
@@ -2230,10 +2108,10 @@
         <v>true</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>401</v>
+        <v>384</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>400</v>
+        <v>383</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2248,15 +2126,15 @@
         <v>true</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>404</v>
+        <v>387</v>
       </c>
       <c r="F3" s="13">
         <f>COUNTIFS(C2:C366,"true")</f>
-        <v>244</v>
+        <v>287</v>
       </c>
       <c r="G3" s="6">
         <f>(F3/365)*100</f>
-        <v>66.849315068493155</v>
+        <v>78.630136986301366</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1">
@@ -2271,15 +2149,15 @@
         <v>true</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>405</v>
+        <v>388</v>
       </c>
       <c r="F4" s="14">
         <f>COUNTIFS(C2:C366,"false")</f>
-        <v>121</v>
+        <v>78</v>
       </c>
       <c r="G4" s="8">
         <f>F4/365*100</f>
-        <v>33.150684931506852</v>
+        <v>21.36986301369863</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1">
@@ -2306,10 +2184,10 @@
         <v>true</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>406</v>
+        <v>389</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>407</v>
+        <v>390</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -2324,11 +2202,11 @@
         <v>true</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>402</v>
+        <v>385</v>
       </c>
       <c r="F7" s="13">
         <f>COUNTIFS(A2:A366,"*peace-related*")</f>
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="G7" s="5">
         <f>COUNTIFS(B2:B366,"*peace-related*")</f>
@@ -2337,21 +2215,21 @@
     </row>
     <row r="8" spans="1:7" ht="15.75" thickBot="1">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>424</v>
       </c>
       <c r="B8" s="19" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
-        <v>true</v>
+        <v>false</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>403</v>
+        <v>386</v>
       </c>
       <c r="F8" s="14">
         <f>COUNTIFS(A2:A366,"*war-related*")</f>
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G8" s="10">
         <f>COUNTIFS(B2:B366,"*war-related*")</f>
@@ -2360,14 +2238,14 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>445</v>
+        <v>7</v>
       </c>
       <c r="B9" s="19" t="s">
         <v>7</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -2384,26 +2262,26 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>458</v>
+        <v>9</v>
       </c>
       <c r="B11" s="19" t="s">
         <v>9</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>425</v>
       </c>
       <c r="B12" s="19" t="s">
         <v>10</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -2420,26 +2298,26 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>491</v>
+        <v>12</v>
       </c>
       <c r="B14" s="19" t="s">
         <v>12</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>426</v>
       </c>
       <c r="B15" s="19" t="s">
         <v>13</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -2492,26 +2370,26 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>427</v>
       </c>
       <c r="B20" s="19" t="s">
         <v>18</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>388</v>
+        <v>19</v>
       </c>
       <c r="B21" s="19" t="s">
         <v>19</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="0"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -2552,7 +2430,7 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>446</v>
+        <v>410</v>
       </c>
       <c r="B25" s="19" t="s">
         <v>23</v>
@@ -2576,7 +2454,7 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>389</v>
+        <v>377</v>
       </c>
       <c r="B27" s="19" t="s">
         <v>25</v>
@@ -2588,38 +2466,38 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>408</v>
+        <v>26</v>
       </c>
       <c r="B28" s="19" t="s">
         <v>26</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="0"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>473</v>
+        <v>27</v>
       </c>
       <c r="B29" s="19" t="s">
         <v>27</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="0"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>383</v>
+        <v>28</v>
       </c>
       <c r="B30" s="19" t="s">
         <v>28</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="0"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -2648,26 +2526,26 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>366</v>
+        <v>31</v>
       </c>
       <c r="B33" s="19" t="s">
         <v>31</v>
       </c>
       <c r="C33" t="str">
         <f t="shared" si="0"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>467</v>
+        <v>32</v>
       </c>
       <c r="B34" s="19" t="s">
         <v>32</v>
       </c>
       <c r="C34" t="str">
         <f t="shared" si="0"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -2780,7 +2658,7 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>409</v>
+        <v>391</v>
       </c>
       <c r="B44" s="19" t="s">
         <v>42</v>
@@ -2864,14 +2742,14 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>367</v>
+        <v>49</v>
       </c>
       <c r="B51" s="19" t="s">
         <v>49</v>
       </c>
       <c r="C51" t="str">
         <f t="shared" si="0"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -2888,14 +2766,14 @@
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>410</v>
+        <v>51</v>
       </c>
       <c r="B53" s="19" t="s">
         <v>51</v>
       </c>
       <c r="C53" t="str">
         <f t="shared" si="0"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -2912,14 +2790,14 @@
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>53</v>
+        <v>428</v>
       </c>
       <c r="B55" s="19" t="s">
         <v>53</v>
       </c>
       <c r="C55" t="str">
         <f t="shared" si="0"/>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -2948,19 +2826,19 @@
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>411</v>
+        <v>56</v>
       </c>
       <c r="B58" s="19" t="s">
         <v>56</v>
       </c>
       <c r="C58" t="str">
         <f t="shared" si="0"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>412</v>
+        <v>392</v>
       </c>
       <c r="B59" s="19" t="s">
         <v>57</v>
@@ -3092,14 +2970,14 @@
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>368</v>
+        <v>68</v>
       </c>
       <c r="B70" s="19" t="s">
         <v>68</v>
       </c>
       <c r="C70" t="str">
         <f t="shared" si="1"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -3116,26 +2994,26 @@
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>70</v>
+        <v>429</v>
       </c>
       <c r="B72" s="19" t="s">
         <v>70</v>
       </c>
       <c r="C72" t="str">
         <f t="shared" si="1"/>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>71</v>
+        <v>430</v>
       </c>
       <c r="B73" s="19" t="s">
         <v>71</v>
       </c>
       <c r="C73" t="str">
         <f t="shared" si="1"/>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -3164,50 +3042,50 @@
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>413</v>
+        <v>74</v>
       </c>
       <c r="B76" s="19" t="s">
         <v>74</v>
       </c>
       <c r="C76" t="str">
         <f t="shared" si="1"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>390</v>
+        <v>75</v>
       </c>
       <c r="B77" s="19" t="s">
         <v>75</v>
       </c>
       <c r="C77" t="str">
         <f t="shared" si="1"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>480</v>
+        <v>76</v>
       </c>
       <c r="B78" s="19" t="s">
         <v>76</v>
       </c>
       <c r="C78" t="str">
         <f t="shared" si="1"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>77</v>
+        <v>431</v>
       </c>
       <c r="B79" s="19" t="s">
         <v>77</v>
       </c>
       <c r="C79" t="str">
         <f t="shared" si="1"/>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -3248,7 +3126,7 @@
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="B83" s="19" t="s">
         <v>81</v>
@@ -3260,7 +3138,7 @@
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>414</v>
+        <v>393</v>
       </c>
       <c r="B84" s="19" t="s">
         <v>82</v>
@@ -3284,26 +3162,26 @@
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>492</v>
+        <v>84</v>
       </c>
       <c r="B86" s="19" t="s">
         <v>84</v>
       </c>
       <c r="C86" t="str">
         <f t="shared" si="1"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>474</v>
+        <v>85</v>
       </c>
       <c r="B87" s="19" t="s">
         <v>85</v>
       </c>
       <c r="C87" t="str">
         <f t="shared" si="1"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -3332,19 +3210,19 @@
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>449</v>
+        <v>88</v>
       </c>
       <c r="B90" s="19" t="s">
         <v>88</v>
       </c>
       <c r="C90" t="str">
         <f t="shared" si="1"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>415</v>
+        <v>394</v>
       </c>
       <c r="B91" s="19" t="s">
         <v>89</v>
@@ -3368,7 +3246,7 @@
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>416</v>
+        <v>395</v>
       </c>
       <c r="B93" s="19" t="s">
         <v>91</v>
@@ -3392,14 +3270,14 @@
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>370</v>
+        <v>93</v>
       </c>
       <c r="B95" s="19" t="s">
         <v>93</v>
       </c>
       <c r="C95" t="str">
         <f t="shared" si="1"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -3464,14 +3342,14 @@
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
-        <v>384</v>
+        <v>99</v>
       </c>
       <c r="B101" s="19" t="s">
         <v>99</v>
       </c>
       <c r="C101" t="str">
         <f t="shared" si="1"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -3500,7 +3378,7 @@
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>417</v>
+        <v>396</v>
       </c>
       <c r="B104" s="19" t="s">
         <v>102</v>
@@ -3536,14 +3414,14 @@
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>475</v>
+        <v>105</v>
       </c>
       <c r="B107" s="19" t="s">
         <v>105</v>
       </c>
       <c r="C107" t="str">
         <f t="shared" si="1"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="108" spans="1:3">
@@ -3560,7 +3438,7 @@
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="B109" s="19" t="s">
         <v>107</v>
@@ -3584,26 +3462,26 @@
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
-        <v>468</v>
+        <v>109</v>
       </c>
       <c r="B111" s="19" t="s">
         <v>109</v>
       </c>
       <c r="C111" t="str">
         <f t="shared" si="1"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
-        <v>462</v>
+        <v>110</v>
       </c>
       <c r="B112" s="19" t="s">
         <v>110</v>
       </c>
       <c r="C112" t="str">
         <f t="shared" si="1"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="113" spans="1:3">
@@ -3644,7 +3522,7 @@
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
-        <v>463</v>
+        <v>413</v>
       </c>
       <c r="B116" s="19" t="s">
         <v>114</v>
@@ -3668,26 +3546,26 @@
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>418</v>
+        <v>116</v>
       </c>
       <c r="B118" s="19" t="s">
         <v>116</v>
       </c>
       <c r="C118" t="str">
         <f t="shared" si="1"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
-        <v>419</v>
+        <v>117</v>
       </c>
       <c r="B119" s="19" t="s">
         <v>117</v>
       </c>
       <c r="C119" t="str">
         <f t="shared" si="1"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -3728,7 +3606,7 @@
     </row>
     <row r="123" spans="1:3">
       <c r="A123" t="s">
-        <v>420</v>
+        <v>397</v>
       </c>
       <c r="B123" s="19" t="s">
         <v>121</v>
@@ -3764,7 +3642,7 @@
     </row>
     <row r="126" spans="1:3">
       <c r="A126" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="B126" s="19" t="s">
         <v>124</v>
@@ -3776,7 +3654,7 @@
     </row>
     <row r="127" spans="1:3">
       <c r="A127" t="s">
-        <v>483</v>
+        <v>418</v>
       </c>
       <c r="B127" s="19" t="s">
         <v>125</v>
@@ -3800,26 +3678,26 @@
     </row>
     <row r="129" spans="1:3">
       <c r="A129" t="s">
-        <v>127</v>
+        <v>432</v>
       </c>
       <c r="B129" s="19" t="s">
         <v>127</v>
       </c>
       <c r="C129" t="str">
         <f t="shared" si="1"/>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="130" spans="1:3">
       <c r="A130" t="s">
-        <v>128</v>
+        <v>433</v>
       </c>
       <c r="B130" s="19" t="s">
         <v>128</v>
       </c>
       <c r="C130" t="str">
         <f t="shared" si="1"/>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="131" spans="1:3">
@@ -3836,31 +3714,31 @@
     </row>
     <row r="132" spans="1:3">
       <c r="A132" t="s">
-        <v>130</v>
+        <v>434</v>
       </c>
       <c r="B132" s="19" t="s">
         <v>130</v>
       </c>
       <c r="C132" t="str">
         <f t="shared" si="2"/>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="133" spans="1:3">
       <c r="A133" t="s">
-        <v>131</v>
+        <v>435</v>
       </c>
       <c r="B133" s="19" t="s">
         <v>131</v>
       </c>
       <c r="C133" t="str">
         <f t="shared" si="2"/>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="134" spans="1:3">
       <c r="A134" t="s">
-        <v>421</v>
+        <v>398</v>
       </c>
       <c r="B134" s="19" t="s">
         <v>132</v>
@@ -3884,7 +3762,7 @@
     </row>
     <row r="136" spans="1:3">
       <c r="A136" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="B136" s="19" t="s">
         <v>134</v>
@@ -3908,31 +3786,31 @@
     </row>
     <row r="138" spans="1:3">
       <c r="A138" t="s">
-        <v>422</v>
+        <v>136</v>
       </c>
       <c r="B138" s="19" t="s">
         <v>136</v>
       </c>
       <c r="C138" t="str">
         <f t="shared" si="2"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="139" spans="1:3">
       <c r="A139" t="s">
-        <v>484</v>
+        <v>137</v>
       </c>
       <c r="B139" s="19" t="s">
         <v>137</v>
       </c>
       <c r="C139" t="str">
         <f t="shared" si="2"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="B140" s="19" t="s">
         <v>138</v>
@@ -3980,7 +3858,7 @@
     </row>
     <row r="144" spans="1:3">
       <c r="A144" t="s">
-        <v>391</v>
+        <v>378</v>
       </c>
       <c r="B144" s="19" t="s">
         <v>142</v>
@@ -3992,7 +3870,7 @@
     </row>
     <row r="145" spans="1:3">
       <c r="A145" t="s">
-        <v>392</v>
+        <v>379</v>
       </c>
       <c r="B145" s="19" t="s">
         <v>143</v>
@@ -4088,26 +3966,26 @@
     </row>
     <row r="153" spans="1:3">
       <c r="A153" t="s">
-        <v>423</v>
+        <v>151</v>
       </c>
       <c r="B153" s="19" t="s">
         <v>151</v>
       </c>
       <c r="C153" t="str">
         <f t="shared" si="2"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="154" spans="1:3">
       <c r="A154" t="s">
-        <v>393</v>
+        <v>152</v>
       </c>
       <c r="B154" s="19" t="s">
         <v>152</v>
       </c>
       <c r="C154" t="str">
         <f t="shared" si="2"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="155" spans="1:3">
@@ -4208,26 +4086,26 @@
     </row>
     <row r="163" spans="1:3">
       <c r="A163" t="s">
-        <v>459</v>
+        <v>161</v>
       </c>
       <c r="B163" s="19" t="s">
         <v>161</v>
       </c>
       <c r="C163" t="str">
         <f t="shared" si="2"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="164" spans="1:3">
       <c r="A164" t="s">
-        <v>162</v>
+        <v>436</v>
       </c>
       <c r="B164" s="19" t="s">
         <v>162</v>
       </c>
       <c r="C164" t="str">
         <f t="shared" si="2"/>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="165" spans="1:3">
@@ -4280,38 +4158,38 @@
     </row>
     <row r="169" spans="1:3">
       <c r="A169" t="s">
-        <v>450</v>
+        <v>167</v>
       </c>
       <c r="B169" s="19" t="s">
         <v>167</v>
       </c>
       <c r="C169" t="str">
         <f t="shared" si="2"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="170" spans="1:3">
       <c r="A170" t="s">
-        <v>375</v>
+        <v>168</v>
       </c>
       <c r="B170" s="19" t="s">
         <v>168</v>
       </c>
       <c r="C170" t="str">
         <f t="shared" si="2"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="171" spans="1:3">
       <c r="A171" t="s">
-        <v>451</v>
+        <v>169</v>
       </c>
       <c r="B171" s="19" t="s">
         <v>169</v>
       </c>
       <c r="C171" t="str">
         <f t="shared" si="2"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="172" spans="1:3">
@@ -4352,7 +4230,7 @@
     </row>
     <row r="175" spans="1:3">
       <c r="A175" t="s">
-        <v>460</v>
+        <v>412</v>
       </c>
       <c r="B175" s="19" t="s">
         <v>173</v>
@@ -4364,7 +4242,7 @@
     </row>
     <row r="176" spans="1:3">
       <c r="A176" t="s">
-        <v>424</v>
+        <v>399</v>
       </c>
       <c r="B176" s="19" t="s">
         <v>174</v>
@@ -4388,7 +4266,7 @@
     </row>
     <row r="178" spans="1:3">
       <c r="A178" t="s">
-        <v>485</v>
+        <v>419</v>
       </c>
       <c r="B178" s="19" t="s">
         <v>176</v>
@@ -4424,26 +4302,26 @@
     </row>
     <row r="181" spans="1:3">
       <c r="A181" t="s">
-        <v>464</v>
+        <v>179</v>
       </c>
       <c r="B181" s="19" t="s">
         <v>179</v>
       </c>
       <c r="C181" t="str">
         <f t="shared" si="2"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="182" spans="1:3">
       <c r="A182" t="s">
-        <v>425</v>
+        <v>180</v>
       </c>
       <c r="B182" s="19" t="s">
         <v>180</v>
       </c>
       <c r="C182" t="str">
         <f t="shared" si="2"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="183" spans="1:3">
@@ -4472,43 +4350,43 @@
     </row>
     <row r="185" spans="1:3">
       <c r="A185" t="s">
-        <v>394</v>
+        <v>183</v>
       </c>
       <c r="B185" s="19" t="s">
         <v>183</v>
       </c>
       <c r="C185" t="str">
         <f t="shared" si="2"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="186" spans="1:3">
       <c r="A186" t="s">
-        <v>426</v>
+        <v>184</v>
       </c>
       <c r="B186" s="19" t="s">
         <v>184</v>
       </c>
       <c r="C186" t="str">
         <f t="shared" si="2"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="187" spans="1:3">
       <c r="A187" t="s">
-        <v>185</v>
+        <v>437</v>
       </c>
       <c r="B187" s="19" t="s">
         <v>185</v>
       </c>
       <c r="C187" t="str">
         <f t="shared" si="2"/>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="188" spans="1:3">
       <c r="A188" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
       <c r="B188" s="19" t="s">
         <v>186</v>
@@ -4532,14 +4410,14 @@
     </row>
     <row r="190" spans="1:3">
       <c r="A190" t="s">
-        <v>427</v>
+        <v>188</v>
       </c>
       <c r="B190" s="19" t="s">
         <v>188</v>
       </c>
       <c r="C190" t="str">
         <f t="shared" si="2"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="191" spans="1:3">
@@ -4580,31 +4458,31 @@
     </row>
     <row r="194" spans="1:3">
       <c r="A194" t="s">
-        <v>376</v>
+        <v>192</v>
       </c>
       <c r="B194" s="19" t="s">
         <v>192</v>
       </c>
       <c r="C194" t="str">
         <f t="shared" si="2"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="195" spans="1:3">
       <c r="A195" t="s">
-        <v>493</v>
+        <v>193</v>
       </c>
       <c r="B195" s="19" t="s">
         <v>193</v>
       </c>
       <c r="C195" t="str">
         <f t="shared" ref="C195:C258" si="3">IF(A195=B195,"true","false")</f>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="196" spans="1:3">
       <c r="A196" t="s">
-        <v>428</v>
+        <v>400</v>
       </c>
       <c r="B196" s="19" t="s">
         <v>194</v>
@@ -4652,7 +4530,7 @@
     </row>
     <row r="200" spans="1:3">
       <c r="A200" t="s">
-        <v>486</v>
+        <v>420</v>
       </c>
       <c r="B200" s="19" t="s">
         <v>198</v>
@@ -4664,19 +4542,19 @@
     </row>
     <row r="201" spans="1:3">
       <c r="A201" t="s">
-        <v>199</v>
+        <v>438</v>
       </c>
       <c r="B201" s="19" t="s">
         <v>199</v>
       </c>
       <c r="C201" t="str">
         <f t="shared" si="3"/>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="202" spans="1:3">
       <c r="A202" t="s">
-        <v>487</v>
+        <v>421</v>
       </c>
       <c r="B202" s="19" t="s">
         <v>200</v>
@@ -4700,7 +4578,7 @@
     </row>
     <row r="204" spans="1:3">
       <c r="A204" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="B204" s="19" t="s">
         <v>202</v>
@@ -4724,14 +4602,14 @@
     </row>
     <row r="206" spans="1:3">
       <c r="A206" t="s">
-        <v>452</v>
+        <v>204</v>
       </c>
       <c r="B206" s="19" t="s">
         <v>204</v>
       </c>
       <c r="C206" t="str">
         <f t="shared" si="3"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="207" spans="1:3">
@@ -4748,7 +4626,7 @@
     </row>
     <row r="208" spans="1:3">
       <c r="A208" t="s">
-        <v>429</v>
+        <v>401</v>
       </c>
       <c r="B208" s="19" t="s">
         <v>206</v>
@@ -4760,26 +4638,26 @@
     </row>
     <row r="209" spans="1:3">
       <c r="A209" t="s">
-        <v>207</v>
+        <v>439</v>
       </c>
       <c r="B209" s="19" t="s">
         <v>207</v>
       </c>
       <c r="C209" t="str">
         <f t="shared" si="3"/>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="210" spans="1:3">
       <c r="A210" t="s">
-        <v>430</v>
+        <v>208</v>
       </c>
       <c r="B210" s="19" t="s">
         <v>208</v>
       </c>
       <c r="C210" t="str">
         <f t="shared" si="3"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="211" spans="1:3">
@@ -4844,7 +4722,7 @@
     </row>
     <row r="216" spans="1:3">
       <c r="A216" t="s">
-        <v>431</v>
+        <v>402</v>
       </c>
       <c r="B216" s="19" t="s">
         <v>214</v>
@@ -4928,7 +4806,7 @@
     </row>
     <row r="223" spans="1:3">
       <c r="A223" t="s">
-        <v>469</v>
+        <v>414</v>
       </c>
       <c r="B223" s="19" t="s">
         <v>221</v>
@@ -4988,26 +4866,26 @@
     </row>
     <row r="228" spans="1:3">
       <c r="A228" t="s">
-        <v>453</v>
+        <v>226</v>
       </c>
       <c r="B228" s="19" t="s">
         <v>226</v>
       </c>
       <c r="C228" t="str">
         <f t="shared" si="3"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="229" spans="1:3">
       <c r="A229" t="s">
-        <v>454</v>
+        <v>227</v>
       </c>
       <c r="B229" s="19" t="s">
         <v>227</v>
       </c>
       <c r="C229" t="str">
         <f t="shared" si="3"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="230" spans="1:3">
@@ -5036,7 +4914,7 @@
     </row>
     <row r="232" spans="1:3">
       <c r="A232" t="s">
-        <v>432</v>
+        <v>403</v>
       </c>
       <c r="B232" s="19" t="s">
         <v>230</v>
@@ -5084,26 +4962,26 @@
     </row>
     <row r="236" spans="1:3">
       <c r="A236" t="s">
-        <v>378</v>
+        <v>234</v>
       </c>
       <c r="B236" s="19" t="s">
         <v>234</v>
       </c>
       <c r="C236" t="str">
         <f t="shared" si="3"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="237" spans="1:3">
       <c r="A237" t="s">
-        <v>433</v>
+        <v>235</v>
       </c>
       <c r="B237" s="19" t="s">
         <v>235</v>
       </c>
       <c r="C237" t="str">
         <f t="shared" si="3"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="238" spans="1:3">
@@ -5120,7 +4998,7 @@
     </row>
     <row r="239" spans="1:3">
       <c r="A239" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
       <c r="B239" s="19" t="s">
         <v>237</v>
@@ -5132,31 +5010,31 @@
     </row>
     <row r="240" spans="1:3">
       <c r="A240" t="s">
-        <v>488</v>
+        <v>238</v>
       </c>
       <c r="B240" s="19" t="s">
         <v>238</v>
       </c>
       <c r="C240" t="str">
         <f t="shared" si="3"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="241" spans="1:3">
       <c r="A241" t="s">
-        <v>455</v>
+        <v>239</v>
       </c>
       <c r="B241" s="19" t="s">
         <v>239</v>
       </c>
       <c r="C241" t="str">
         <f t="shared" si="3"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="242" spans="1:3">
       <c r="A242" t="s">
-        <v>434</v>
+        <v>404</v>
       </c>
       <c r="B242" s="19" t="s">
         <v>240</v>
@@ -5168,14 +5046,14 @@
     </row>
     <row r="243" spans="1:3">
       <c r="A243" t="s">
-        <v>241</v>
+        <v>440</v>
       </c>
       <c r="B243" s="19" t="s">
         <v>241</v>
       </c>
       <c r="C243" t="str">
         <f t="shared" si="3"/>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="244" spans="1:3">
@@ -5204,26 +5082,26 @@
     </row>
     <row r="246" spans="1:3">
       <c r="A246" t="s">
-        <v>476</v>
+        <v>244</v>
       </c>
       <c r="B246" s="19" t="s">
         <v>244</v>
       </c>
       <c r="C246" t="str">
         <f t="shared" si="3"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="247" spans="1:3">
       <c r="A247" t="s">
-        <v>245</v>
+        <v>441</v>
       </c>
       <c r="B247" s="19" t="s">
         <v>245</v>
       </c>
       <c r="C247" t="str">
         <f t="shared" si="3"/>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="248" spans="1:3">
@@ -5240,14 +5118,14 @@
     </row>
     <row r="249" spans="1:3">
       <c r="A249" t="s">
-        <v>456</v>
+        <v>247</v>
       </c>
       <c r="B249" s="19" t="s">
         <v>247</v>
       </c>
       <c r="C249" t="str">
         <f t="shared" si="3"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="250" spans="1:3">
@@ -5276,14 +5154,14 @@
     </row>
     <row r="252" spans="1:3">
       <c r="A252" t="s">
-        <v>250</v>
+        <v>442</v>
       </c>
       <c r="B252" s="19" t="s">
         <v>250</v>
       </c>
       <c r="C252" t="str">
         <f t="shared" si="3"/>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="253" spans="1:3">
@@ -5300,14 +5178,14 @@
     </row>
     <row r="254" spans="1:3">
       <c r="A254" t="s">
-        <v>252</v>
+        <v>443</v>
       </c>
       <c r="B254" s="19" t="s">
         <v>252</v>
       </c>
       <c r="C254" t="str">
         <f t="shared" si="3"/>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="255" spans="1:3">
@@ -5324,7 +5202,7 @@
     </row>
     <row r="256" spans="1:3">
       <c r="A256" t="s">
-        <v>435</v>
+        <v>405</v>
       </c>
       <c r="B256" s="19" t="s">
         <v>254</v>
@@ -5336,14 +5214,14 @@
     </row>
     <row r="257" spans="1:3">
       <c r="A257" t="s">
-        <v>255</v>
+        <v>444</v>
       </c>
       <c r="B257" s="19" t="s">
         <v>255</v>
       </c>
       <c r="C257" t="str">
         <f t="shared" si="3"/>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="258" spans="1:3">
@@ -5408,19 +5286,19 @@
     </row>
     <row r="263" spans="1:3">
       <c r="A263" t="s">
-        <v>436</v>
+        <v>261</v>
       </c>
       <c r="B263" s="19" t="s">
         <v>261</v>
       </c>
       <c r="C263" t="str">
         <f t="shared" si="4"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="264" spans="1:3">
       <c r="A264" t="s">
-        <v>437</v>
+        <v>406</v>
       </c>
       <c r="B264" s="19" t="s">
         <v>262</v>
@@ -5492,74 +5370,74 @@
     </row>
     <row r="270" spans="1:3">
       <c r="A270" t="s">
-        <v>268</v>
+        <v>445</v>
       </c>
       <c r="B270" s="19" t="s">
         <v>268</v>
       </c>
       <c r="C270" t="str">
         <f t="shared" si="4"/>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="271" spans="1:3">
       <c r="A271" t="s">
-        <v>477</v>
+        <v>269</v>
       </c>
       <c r="B271" s="19" t="s">
         <v>269</v>
       </c>
       <c r="C271" t="str">
         <f t="shared" si="4"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="272" spans="1:3">
       <c r="A272" t="s">
-        <v>270</v>
+        <v>446</v>
       </c>
       <c r="B272" s="19" t="s">
         <v>270</v>
       </c>
       <c r="C272" t="str">
         <f t="shared" si="4"/>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="273" spans="1:3">
       <c r="A273" t="s">
-        <v>478</v>
+        <v>271</v>
       </c>
       <c r="B273" s="19" t="s">
         <v>271</v>
       </c>
       <c r="C273" t="str">
         <f t="shared" si="4"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="274" spans="1:3">
       <c r="A274" t="s">
-        <v>272</v>
+        <v>447</v>
       </c>
       <c r="B274" s="19" t="s">
         <v>272</v>
       </c>
       <c r="C274" t="str">
         <f t="shared" si="4"/>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="275" spans="1:3">
       <c r="A275" t="s">
-        <v>457</v>
+        <v>273</v>
       </c>
       <c r="B275" s="19" t="s">
         <v>273</v>
       </c>
       <c r="C275" t="str">
         <f t="shared" si="4"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="276" spans="1:3">
@@ -5588,14 +5466,14 @@
     </row>
     <row r="278" spans="1:3">
       <c r="A278" t="s">
-        <v>396</v>
+        <v>276</v>
       </c>
       <c r="B278" s="19" t="s">
         <v>276</v>
       </c>
       <c r="C278" t="str">
         <f t="shared" si="4"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="279" spans="1:3">
@@ -5612,19 +5490,19 @@
     </row>
     <row r="280" spans="1:3">
       <c r="A280" t="s">
-        <v>278</v>
+        <v>448</v>
       </c>
       <c r="B280" s="19" t="s">
         <v>278</v>
       </c>
       <c r="C280" t="str">
         <f t="shared" si="4"/>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="281" spans="1:3">
       <c r="A281" t="s">
-        <v>399</v>
+        <v>382</v>
       </c>
       <c r="B281" s="19" t="s">
         <v>279</v>
@@ -5672,7 +5550,7 @@
     </row>
     <row r="285" spans="1:3">
       <c r="A285" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
       <c r="B285" s="19" t="s">
         <v>283</v>
@@ -5720,7 +5598,7 @@
     </row>
     <row r="289" spans="1:3">
       <c r="A289" t="s">
-        <v>489</v>
+        <v>422</v>
       </c>
       <c r="B289" s="19" t="s">
         <v>287</v>
@@ -5756,26 +5634,26 @@
     </row>
     <row r="292" spans="1:3">
       <c r="A292" t="s">
-        <v>290</v>
+        <v>449</v>
       </c>
       <c r="B292" s="19" t="s">
         <v>290</v>
       </c>
       <c r="C292" t="str">
         <f t="shared" si="4"/>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="293" spans="1:3">
       <c r="A293" t="s">
-        <v>470</v>
+        <v>291</v>
       </c>
       <c r="B293" s="19" t="s">
         <v>291</v>
       </c>
       <c r="C293" t="str">
         <f t="shared" si="4"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="294" spans="1:3">
@@ -5792,26 +5670,26 @@
     </row>
     <row r="295" spans="1:3">
       <c r="A295" t="s">
-        <v>494</v>
+        <v>293</v>
       </c>
       <c r="B295" s="19" t="s">
         <v>293</v>
       </c>
       <c r="C295" t="str">
         <f t="shared" si="4"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="296" spans="1:3">
       <c r="A296" t="s">
-        <v>294</v>
+        <v>450</v>
       </c>
       <c r="B296" s="19" t="s">
         <v>294</v>
       </c>
       <c r="C296" t="str">
         <f t="shared" si="4"/>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="297" spans="1:3">
@@ -5852,7 +5730,7 @@
     </row>
     <row r="300" spans="1:3">
       <c r="A300" t="s">
-        <v>438</v>
+        <v>407</v>
       </c>
       <c r="B300" s="19" t="s">
         <v>298</v>
@@ -5888,7 +5766,7 @@
     </row>
     <row r="303" spans="1:3">
       <c r="A303" t="s">
-        <v>481</v>
+        <v>417</v>
       </c>
       <c r="B303" s="19" t="s">
         <v>301</v>
@@ -5912,7 +5790,7 @@
     </row>
     <row r="305" spans="1:3">
       <c r="A305" t="s">
-        <v>495</v>
+        <v>423</v>
       </c>
       <c r="B305" s="19" t="s">
         <v>303</v>
@@ -5924,7 +5802,7 @@
     </row>
     <row r="306" spans="1:3">
       <c r="A306" t="s">
-        <v>439</v>
+        <v>408</v>
       </c>
       <c r="B306" s="19" t="s">
         <v>304</v>
@@ -5960,26 +5838,26 @@
     </row>
     <row r="309" spans="1:3">
       <c r="A309" t="s">
-        <v>379</v>
+        <v>307</v>
       </c>
       <c r="B309" s="19" t="s">
         <v>307</v>
       </c>
       <c r="C309" t="str">
         <f t="shared" si="4"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="310" spans="1:3">
       <c r="A310" t="s">
-        <v>482</v>
+        <v>308</v>
       </c>
       <c r="B310" s="19" t="s">
         <v>308</v>
       </c>
       <c r="C310" t="str">
         <f t="shared" si="4"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="311" spans="1:3">
@@ -5996,26 +5874,26 @@
     </row>
     <row r="312" spans="1:3">
       <c r="A312" t="s">
-        <v>310</v>
+        <v>451</v>
       </c>
       <c r="B312" s="19" t="s">
         <v>310</v>
       </c>
       <c r="C312" t="str">
         <f t="shared" si="4"/>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="313" spans="1:3">
       <c r="A313" t="s">
-        <v>440</v>
+        <v>311</v>
       </c>
       <c r="B313" s="19" t="s">
         <v>311</v>
       </c>
       <c r="C313" t="str">
         <f t="shared" si="4"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="314" spans="1:3">
@@ -6044,7 +5922,7 @@
     </row>
     <row r="316" spans="1:3">
       <c r="A316" t="s">
-        <v>471</v>
+        <v>415</v>
       </c>
       <c r="B316" s="19" t="s">
         <v>314</v>
@@ -6092,31 +5970,31 @@
     </row>
     <row r="320" spans="1:3">
       <c r="A320" t="s">
-        <v>465</v>
+        <v>318</v>
       </c>
       <c r="B320" s="19" t="s">
         <v>318</v>
       </c>
       <c r="C320" t="str">
         <f t="shared" si="4"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="321" spans="1:3">
       <c r="A321" t="s">
-        <v>461</v>
+        <v>319</v>
       </c>
       <c r="B321" s="19" t="s">
         <v>319</v>
       </c>
       <c r="C321" t="str">
         <f t="shared" si="4"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="322" spans="1:3">
       <c r="A322" t="s">
-        <v>441</v>
+        <v>409</v>
       </c>
       <c r="B322" s="19" t="s">
         <v>320</v>
@@ -6224,14 +6102,14 @@
     </row>
     <row r="331" spans="1:3">
       <c r="A331" t="s">
-        <v>329</v>
+        <v>452</v>
       </c>
       <c r="B331" s="19" t="s">
         <v>329</v>
       </c>
       <c r="C331" t="str">
         <f t="shared" si="5"/>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="332" spans="1:3">
@@ -6260,26 +6138,26 @@
     </row>
     <row r="334" spans="1:3">
       <c r="A334" t="s">
-        <v>442</v>
+        <v>332</v>
       </c>
       <c r="B334" s="19" t="s">
         <v>332</v>
       </c>
       <c r="C334" t="str">
         <f t="shared" si="5"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="335" spans="1:3">
       <c r="A335" t="s">
-        <v>397</v>
+        <v>333</v>
       </c>
       <c r="B335" s="19" t="s">
         <v>333</v>
       </c>
       <c r="C335" t="str">
         <f t="shared" si="5"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="336" spans="1:3">
@@ -6332,14 +6210,14 @@
     </row>
     <row r="340" spans="1:3">
       <c r="A340" t="s">
-        <v>443</v>
+        <v>338</v>
       </c>
       <c r="B340" s="19" t="s">
         <v>338</v>
       </c>
       <c r="C340" t="str">
         <f t="shared" si="5"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="341" spans="1:3">
@@ -6368,19 +6246,19 @@
     </row>
     <row r="343" spans="1:3">
       <c r="A343" t="s">
-        <v>466</v>
+        <v>341</v>
       </c>
       <c r="B343" s="19" t="s">
         <v>341</v>
       </c>
       <c r="C343" t="str">
         <f t="shared" si="5"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="344" spans="1:3">
       <c r="A344" t="s">
-        <v>479</v>
+        <v>416</v>
       </c>
       <c r="B344" s="19" t="s">
         <v>342</v>
@@ -6404,7 +6282,7 @@
     </row>
     <row r="346" spans="1:3">
       <c r="A346" t="s">
-        <v>447</v>
+        <v>411</v>
       </c>
       <c r="B346" s="19" t="s">
         <v>344</v>
@@ -6440,26 +6318,26 @@
     </row>
     <row r="349" spans="1:3">
       <c r="A349" t="s">
-        <v>496</v>
+        <v>347</v>
       </c>
       <c r="B349" s="19" t="s">
         <v>347</v>
       </c>
       <c r="C349" t="str">
         <f t="shared" si="5"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="350" spans="1:3">
       <c r="A350" t="s">
-        <v>348</v>
+        <v>453</v>
       </c>
       <c r="B350" s="19" t="s">
         <v>348</v>
       </c>
       <c r="C350" t="str">
         <f t="shared" si="5"/>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="351" spans="1:3">
@@ -6488,7 +6366,7 @@
     </row>
     <row r="353" spans="1:3">
       <c r="A353" t="s">
-        <v>398</v>
+        <v>381</v>
       </c>
       <c r="B353" s="19" t="s">
         <v>351</v>
@@ -6512,14 +6390,14 @@
     </row>
     <row r="355" spans="1:3">
       <c r="A355" t="s">
-        <v>387</v>
+        <v>353</v>
       </c>
       <c r="B355" s="19" t="s">
         <v>353</v>
       </c>
       <c r="C355" t="str">
         <f t="shared" si="5"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="356" spans="1:3">
@@ -6548,26 +6426,26 @@
     </row>
     <row r="358" spans="1:3">
       <c r="A358" t="s">
-        <v>490</v>
+        <v>356</v>
       </c>
       <c r="B358" s="19" t="s">
         <v>356</v>
       </c>
       <c r="C358" t="str">
         <f t="shared" si="5"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="359" spans="1:3">
       <c r="A359" t="s">
-        <v>472</v>
+        <v>357</v>
       </c>
       <c r="B359" s="19" t="s">
         <v>357</v>
       </c>
       <c r="C359" t="str">
         <f t="shared" si="5"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="360" spans="1:3">
@@ -6596,14 +6474,14 @@
     </row>
     <row r="362" spans="1:3">
       <c r="A362" t="s">
-        <v>448</v>
+        <v>360</v>
       </c>
       <c r="B362" s="19" t="s">
         <v>360</v>
       </c>
       <c r="C362" t="str">
         <f t="shared" si="5"/>
-        <v>false</v>
+        <v>true</v>
       </c>
     </row>
     <row r="363" spans="1:3">
@@ -6644,26 +6522,31 @@
     </row>
     <row r="366" spans="1:3">
       <c r="A366" t="s">
-        <v>444</v>
+        <v>364</v>
       </c>
       <c r="B366" s="19" t="s">
         <v>364</v>
       </c>
       <c r="C366" t="str">
         <f t="shared" si="5"/>
-        <v>false</v>
+        <v>true</v>
+      </c>
+    </row>
+    <row r="367" spans="1:3">
+      <c r="A367" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="368" spans="1:3">
       <c r="C368" s="2">
         <f>COUNTIFS(C2:C366,"true")</f>
-        <v>244</v>
+        <v>287</v>
       </c>
     </row>
     <row r="369" spans="3:3">
       <c r="C369" s="3">
         <f>COUNTIFS(C2:C366,"false")</f>
-        <v>121</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added pptx, readme, run.sh
</commit_message>
<xml_diff>
--- a/files/output/Comparison_FPROG.xlsx
+++ b/files/output/Comparison_FPROG.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fhtw-my.sharepoint.com/personal/if21b028_technikum-wien_at/Documents/INFORMATIK/Semester 5/FPROG/project/FPROG/files/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="118" documentId="8_{BBED4159-DCCB-4A4C-8A89-83957CA5B522}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{804DBE43-B364-41CE-AD53-A7886D5EF1CD}"/>
+  <xr:revisionPtr revIDLastSave="119" documentId="8_{BBED4159-DCCB-4A4C-8A89-83957CA5B522}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE3D19A4-2C20-4943-9137-013B2750C5EC}"/>
   <bookViews>
-    <workbookView xWindow="3495" yWindow="960" windowWidth="21600" windowHeight="11385" xr2:uid="{CD60B827-A9D0-4185-BC28-64C39489518C}"/>
+    <workbookView minimized="1" xWindow="3495" yWindow="960" windowWidth="21600" windowHeight="11385" xr2:uid="{CD60B827-A9D0-4185-BC28-64C39489518C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -2074,7 +2074,7 @@
   <dimension ref="A1:G369"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>